<commit_message>
change FK PollingStation on Station in Friends, update frontEnd
</commit_message>
<xml_diff>
--- a/UploadFriends.xlsx
+++ b/UploadFriends.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
   <si>
     <t>FamilyName</t>
   </si>
@@ -82,15 +82,9 @@
     <t>Кремль</t>
   </si>
   <si>
-    <t>Промышленность</t>
-  </si>
-  <si>
     <t>01.01.2021</t>
   </si>
   <si>
-    <t>Да</t>
-  </si>
-  <si>
     <t>Нет описания</t>
   </si>
   <si>
@@ -157,9 +151,6 @@
     <t>Группа</t>
   </si>
   <si>
-    <t>UIS</t>
-  </si>
-  <si>
     <t>01.01.1978</t>
   </si>
   <si>
@@ -206,9 +197,6 @@
   </si>
   <si>
     <t>3215</t>
-  </si>
-  <si>
-    <t>1001</t>
   </si>
   <si>
     <t>+79225353972</t>
@@ -277,12 +265,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -298,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -313,6 +313,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -620,57 +632,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="11"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
     <col min="10" max="10" width="19.7109375" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" style="15" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" style="11" customWidth="1"/>
     <col min="16" max="16" width="25" customWidth="1"/>
     <col min="17" max="17" width="19.42578125" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" customWidth="1"/>
     <col min="19" max="19" width="12.7109375" customWidth="1"/>
     <col min="20" max="20" width="7.85546875" style="2" customWidth="1"/>
     <col min="21" max="21" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -680,18 +693,18 @@
         <v>8</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" s="12" t="s">
         <v>9</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="3" t="s">
@@ -707,286 +720,253 @@
         <v>15</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="V2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="D3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="10">
         <v>10</v>
       </c>
       <c r="I3" s="2">
         <v>33</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="2">
-        <v>1001</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="M3" s="14"/>
       <c r="N3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="O3" s="10"/>
       <c r="P3" s="2">
         <v>89225353971</v>
       </c>
       <c r="Q3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="D4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="10">
         <v>10</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="14"/>
       <c r="N4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="O4" s="10"/>
       <c r="P4" s="2">
         <v>89225353972</v>
       </c>
       <c r="Q4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="U4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="V4" s="2"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="10">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="2">
-        <v>10</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="14"/>
       <c r="N5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="O5" s="10"/>
       <c r="P5" s="2">
         <v>89225353973</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="S5" s="2"/>
       <c r="T5" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="V5" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
update upload from json
</commit_message>
<xml_diff>
--- a/UploadFriends.xlsx
+++ b/UploadFriends.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Freinds" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
   <si>
     <t>FamilyName</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Дмитрий</t>
   </si>
   <si>
-    <t>Оренбург</t>
-  </si>
-  <si>
     <t>Советская</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>3215</t>
   </si>
   <si>
-    <t>+79225353972</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -217,9 +211,6 @@
     <t>Ивановна</t>
   </si>
   <si>
-    <t>+79225353973</t>
-  </si>
-  <si>
     <t>anna@mail.ru</t>
   </si>
   <si>
@@ -233,6 +224,24 @@
   </si>
   <si>
     <t>Избирательный округ</t>
+  </si>
+  <si>
+    <t>89225353973</t>
+  </si>
+  <si>
+    <t>++89225353972</t>
+  </si>
+  <si>
+    <t>+7922-5353-972</t>
+  </si>
+  <si>
+    <t>1009</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>222</t>
   </si>
 </sst>
 </file>
@@ -298,7 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -325,6 +334,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -632,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,10 +703,10 @@
         <v>8</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>9</v>
@@ -720,13 +730,13 @@
         <v>15</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -734,90 +744,88 @@
         <v>17</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="V2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>20</v>
       </c>
       <c r="H3" s="10">
         <v>10</v>
@@ -826,145 +834,147 @@
         <v>33</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="M3" s="14"/>
+        <v>53</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="N3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O3" s="10"/>
       <c r="P3" s="2">
         <v>89225353971</v>
       </c>
       <c r="Q3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>20</v>
       </c>
       <c r="H4" s="10">
         <v>10</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L4" s="2"/>
-      <c r="M4" s="14"/>
+      <c r="M4" s="14" t="s">
+        <v>74</v>
+      </c>
       <c r="N4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="2">
-        <v>89225353972</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="R4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V4" s="2"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>20</v>
       </c>
       <c r="H5" s="10">
         <v>10</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="K5" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="14"/>
+      <c r="M5" s="14" t="s">
+        <v>75</v>
+      </c>
       <c r="N5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O5" s="10"/>
       <c r="P5" s="2">
         <v>89225353973</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V5" s="2"/>
     </row>

</xml_diff>